<commit_message>
fix: Parameters for components and regenerated outputs
</commit_message>
<xml_diff>
--- a/Altium Design/ADA2/Project Outputs for ADA2/BOM/Bill of Materials.xlsx
+++ b/Altium Design/ADA2/Project Outputs for ADA2/BOM/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idiaz\Desktop\FlightComputer\Altium Design\ADA2\Project Outputs for ADA2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74B7F565-3F6A-479F-81EB-DED6A91C9459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFEA3E51-C38B-47C7-8BD8-9BDDBBF5DA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="1260" windowWidth="15300" windowHeight="7785"/>
   </bookViews>
@@ -39,23 +39,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="155">
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Designator</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Manufacturer Part Number</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -65,13 +65,133 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Capacitor SMD 4.7nF, ESD Suppressors / TVS Diodes Single Line Transil Vbr 5V min 26pF 0, Red, Green, Blue _RGB_ 622nm Red, 530nm Green, 470nm Blue LED Indication - Discrete 1.9V Red, 3V Green, 3V Blue 4-PLCC, LED SMD Verde, FIDUCIAL, [NoValue], Header, 6-Pin, USB - micro B USB 2.0 Receptacle Connector 5 Position Surface Mount, Right Angle; Through Hole, Connector Header Surface Mount 2 position 0.049 (1.25mm), Resistencia SMD 470ohms, Bluetooth, WiFi 802.11b/g/n, Bluetooth v4.2 +EDR, Class 1, 2 and 3 Transceiver Module 2.4GHz ~ 2.5GHz Integrated, Trace Surface Mount, MPU-6050 series Accelerometer, Gyroscope, 3 Axis Sensor Evaluation Board, USB Interface IC USB to UART bridge - QFN28, 8M-bit 3.0V Serial Flash Memory with uniform 4KB sectors and Dual/Quad SPI, Board Mount Pressure Sensors, 500-mA, low-noise, low-IQ, low-dropout voltage regulator with reverse current protection 6-WSON -40 to 125</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, D1, D2, D3, D4, D5, D6, FD1, FD2, FD3, H1, H3, H4, P3, P4, P5, P6, P7, P8, Q3, R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, U1, U2, U3, U4, U5, U6</t>
-  </si>
-  <si>
-    <t/>
+    <t>C1, C10, C13, C15, C19, C21</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>FH (Guangdong Fenghua Advanced Tech)</t>
+  </si>
+  <si>
+    <t>0805F105Z250NT</t>
+  </si>
+  <si>
+    <t>Capacitor SMD 4.7nF</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>C285184</t>
+  </si>
+  <si>
+    <t>C2, C16</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL21A226KPCLRNC</t>
+  </si>
+  <si>
+    <t>C318688</t>
+  </si>
+  <si>
+    <t>C3, C4, C5, C6, C7, C9, C12, C14, C17, C18, C20</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>0805B104M500NT</t>
+  </si>
+  <si>
+    <t>C286511</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>2.2nF</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CC0805JRX7R0BB222</t>
+  </si>
+  <si>
+    <t>C527219</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>PSA(Prosperity Dielectrics)</t>
+  </si>
+  <si>
+    <t>FN21X103K500PXG</t>
+  </si>
+  <si>
+    <t>C525298</t>
+  </si>
+  <si>
+    <t>D1, D2, D3</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>ESDALC5-1BT2Y</t>
+  </si>
+  <si>
+    <t>ESD Suppressors / TVS Diodes Single Line Transil Vbr 5V min 26pF 0</t>
+  </si>
+  <si>
+    <t>C3712112</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>CREELED, INC.</t>
+  </si>
+  <si>
+    <t>CLVBA-FKA-CAEDH8BBB7A363</t>
+  </si>
+  <si>
+    <t>Red, Green, Blue _RGB_ 622nm Red, 530nm Green, 470nm Blue LED Indication - Discrete 1.9V Red, 3V Green, 3V Blue 4-PLCC</t>
+  </si>
+  <si>
+    <t>C5250259</t>
+  </si>
+  <si>
+    <t>D5, D6</t>
+  </si>
+  <si>
+    <t>Everlight Elec</t>
+  </si>
+  <si>
+    <t>19-217/R6C-AL1M2VY/3T</t>
+  </si>
+  <si>
+    <t>LED SMD Verde</t>
+  </si>
+  <si>
+    <t>C72044</t>
+  </si>
+  <si>
+    <t>FD1, FD2, FD3, H1, H3, H4</t>
+  </si>
+  <si>
+    <t>FIDUCIAL, [NoValue]</t>
   </si>
   <si>
     <t>P1, P2</t>
@@ -83,12 +203,69 @@
     <t>PZ254V-11-05P</t>
   </si>
   <si>
-    <t>JLCPCB</t>
+    <t>Straight Square Pins 2.5mm 6mm -40℃~+105℃ 3mm 5 2.54mm 单排 Black Brass 1x5P Plugin,P=2.54mm  Pin Headers ROHS</t>
   </si>
   <si>
     <t>C492404</t>
   </si>
   <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>PZ254V-11-06P</t>
+  </si>
+  <si>
+    <t>Header, 6-Pin</t>
+  </si>
+  <si>
+    <t>C492405</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>1050170001</t>
+  </si>
+  <si>
+    <t>USB - micro B USB 2.0 Receptacle Connector 5 Position Surface Mount, Right Angle; Through Hole</t>
+  </si>
+  <si>
+    <t>C136000</t>
+  </si>
+  <si>
+    <t>P5, P6, P8</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>1727010</t>
+  </si>
+  <si>
+    <t>13.5A 200V Green Straight pin 3.81mm 1 2 Plugin,P=3.81mm  Screw terminal ROHS</t>
+  </si>
+  <si>
+    <t>C89123</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>JST Sales America</t>
+  </si>
+  <si>
+    <t>BM02B-GHS-TBT(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount 2 position 0.049 (1.25mm)</t>
+  </si>
+  <si>
+    <t>C161690</t>
+  </si>
+  <si>
     <t>Q1, Q2</t>
   </si>
   <si>
@@ -98,37 +275,235 @@
     <t>S8050</t>
   </si>
   <si>
+    <t>25V 300mW 500mA SOT-23  Bipolar Transistors - BJT ROHS</t>
+  </si>
+  <si>
     <t>C916390</t>
   </si>
   <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Taiwan Semiconductor Corporation</t>
+  </si>
+  <si>
+    <t>TSM200N03DPQ33 RGG</t>
+  </si>
+  <si>
+    <t>MOSFET 2 N-CH 30V 20A 8PDFN</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>TSM200N03DPQ33RGGCT-ND</t>
+  </si>
+  <si>
+    <t>R1, R10, R13, R16, R17, R19, R20</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
+    <t>CQ05W8J0471T5E</t>
+  </si>
+  <si>
+    <t>Resistencia SMD 470ohms</t>
+  </si>
+  <si>
+    <t>C473621</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R5, R6, R7, R8, R9, R14, R15</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>Viking Tech</t>
+  </si>
+  <si>
+    <t>ARG05BTC1002</t>
+  </si>
+  <si>
+    <t>C406725</t>
+  </si>
+  <si>
+    <t>R11, R12</t>
+  </si>
+  <si>
+    <t>4K7</t>
+  </si>
+  <si>
+    <t>CR-05FL7---4K7</t>
+  </si>
+  <si>
+    <t>C280006</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>RC0805FR-071ML</t>
+  </si>
+  <si>
+    <t>C107700</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>22K</t>
+  </si>
+  <si>
+    <t>KOA Speer Elec</t>
+  </si>
+  <si>
+    <t>RN73H2ATTD2202B25</t>
+  </si>
+  <si>
+    <t>C186285</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>47K</t>
+  </si>
+  <si>
+    <t>Sunway</t>
+  </si>
+  <si>
+    <t>SC0805J4702F4ANRH</t>
+  </si>
+  <si>
+    <t>C3152235</t>
+  </si>
+  <si>
+    <t>S1, S2</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>PTS645SM43SMTR92LFS</t>
+  </si>
+  <si>
     <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
   </si>
   <si>
-    <t>S1, S2</t>
-  </si>
-  <si>
-    <t>C&amp;K</t>
-  </si>
-  <si>
-    <t>PTS645SM43SMTR92LFS</t>
-  </si>
-  <si>
     <t>C221880</t>
   </si>
   <si>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6</t>
+  </si>
+  <si>
+    <t>Ronghe</t>
+  </si>
+  <si>
+    <t>RH-5015</t>
+  </si>
+  <si>
     <t>Thimble/Copper Rod/Test Ring ROHS</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6</t>
-  </si>
-  <si>
-    <t>Ronghe</t>
-  </si>
-  <si>
-    <t>RH-5015</t>
-  </si>
-  <si>
     <t>C5199798</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Espressif Systems</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32E-N16</t>
+  </si>
+  <si>
+    <t>Bluetooth, WiFi 802.11b/g/n, Bluetooth v4.2 +EDR, Class 1, 2 and 3 Transceiver Module 2.4GHz ~ 2.5GHz Integrated, Trace Surface Mount</t>
+  </si>
+  <si>
+    <t>C701343</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TDK InvenSense</t>
+  </si>
+  <si>
+    <t>MPU-6050</t>
+  </si>
+  <si>
+    <t>MPU-6050 series Accelerometer, Gyroscope, 3 Axis Sensor Evaluation Board</t>
+  </si>
+  <si>
+    <t>C24112</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SILICON LABS</t>
+  </si>
+  <si>
+    <t>CP2102N-A02-GQFN28R</t>
+  </si>
+  <si>
+    <t>USB Interface IC USB to UART bridge - QFN28</t>
+  </si>
+  <si>
+    <t>C964632</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Winbond Elec</t>
+  </si>
+  <si>
+    <t>W25Q80DVSSIG</t>
+  </si>
+  <si>
+    <t>8M-bit 3.0V Serial Flash Memory with uniform 4KB sectors and Dual/Quad SPI</t>
+  </si>
+  <si>
+    <t>C14086</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>BOSCH</t>
+  </si>
+  <si>
+    <t>BMP390</t>
+  </si>
+  <si>
+    <t>Board Mount Pressure Sensors</t>
+  </si>
+  <si>
+    <t>C5124834</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>LP5912-3.3DRVT</t>
+  </si>
+  <si>
+    <t>500-mA, low-noise, low-IQ, low-dropout voltage regulator with reverse current protection 6-WSON -40 to 125</t>
+  </si>
+  <si>
+    <t>C134121</t>
   </si>
 </sst>
 </file>
@@ -505,14 +880,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="7" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -552,33 +929,43 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="H2" s="1">
-        <v>68</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
@@ -586,74 +973,684 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="D21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="1">
         <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>